<commit_message>
Updated customer delete logic and fixed typos
</commit_message>
<xml_diff>
--- a/Sample_Customer_List.xlsx
+++ b/Sample_Customer_List.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,177 +471,229 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1001</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1002</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rahul Sharma</t>
+          <t>Priya Verma</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Flat 101, Galaxy Apts, Nagpur</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>9876543210</t>
-        </is>
+          <t>Plot 45, Shivaji Nagar, Nagpur</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>9123456789</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>STB-998877</t>
+          <t>STB-112233</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>650</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1002</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1003</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Priya Verma</t>
+          <t>Amitabh Patel</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Plot 45, Shivaji Nagar, Nagpur</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>9123456789</t>
-        </is>
+          <t>12, Main Road, Jaripatka</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>9988776655</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>STB-112233</t>
+          <t>STB-445566</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
+          <t>2025-12-10</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>400</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1003</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1004</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Amitabh Patel</t>
+          <t>Sneha Gupta</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12, Main Road, Jaripatka</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>9988776655</t>
-        </is>
+          <t>B-Wing, Sunrise Society, Sadar</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>9000011111</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>STB-445566</t>
+          <t>STB-778899</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
+          <t>2025-12-15</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1004</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1005</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sneha Gupta</t>
+          <t>Vikram Singh</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>B-Wing, Sunrise Society, Sadar</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>9000011111</t>
-        </is>
+          <t>Near Old Temple, Mahal</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>8888822222</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>STB-778899</t>
+          <t>STB-000000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+          <t>2025-12-20</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1005</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>6654</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Vikram Singh</t>
+          <t>rahul verma</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Near Old Temple, Mahal</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>8888822222</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>STB-000000</t>
-        </is>
+          <t>nagpore</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>645451</v>
+      </c>
+      <c r="E6" t="n">
+        <v>616546546</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>2025-12-20</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>500</t>
+      <c r="G6" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>65541654</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Rahul Kumar</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>12 koli</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>264768446</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>68146545314661</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>23436854</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Rahul Sharma</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10 no puliya</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>987845665</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>234143434788</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-12-15</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>